<commit_message>
default_cache_value config feature; cells referred to via a named range don't auto cast for SUM(namedRange)
</commit_message>
<xml_diff>
--- a/xls/baremetrics_plan1.xlsx
+++ b/xls/baremetrics_plan1.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="1"/>
@@ -11,7 +11,7 @@
     <sheet name="data" sheetId="3" r:id="rId2"/>
     <sheet name="s2cfg" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725" calcOnSave="0"/>
+  <calcPr calcId="145621" calcOnSave="0"/>
 </workbook>
 </file>
 
@@ -51,9 +51,6 @@
     <t>planQuery1</t>
   </si>
   <si>
-    <t>plan</t>
-  </si>
-  <si>
     <t>plan.name</t>
   </si>
   <si>
@@ -64,16 +61,19 @@
   </si>
   <si>
     <t>plan.amounts.0.amount</t>
+  </si>
+  <si>
+    <t>plans</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -123,15 +123,17 @@
 <file path=xl/volatileDependencies.xml><?xml version="1.0" encoding="utf-8"?>
 <volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <volType type="realTimeData">
-    <main first="rtdsrv.333b7e2519fb440d9688e2cbd7e8feed">
+    <main first="rtdsrv.49b4396a38154ab791cc3f1ac4995a8a">
       <tp t="s">
         <v>complete</v>
         <stp/>
         <stp>baremetrics.planQuery1.status</stp>
         <tr r="B3" s="1"/>
       </tp>
+    </main>
+    <main first="rtdsrv.49b4396a38154ab791cc3f1ac4995a8a">
       <tp t="s">
-        <v>18</v>
+        <v>20</v>
         <stp/>
         <stp>baremetrics.planQuery1.count</stp>
         <tr r="B2" s="1"/>
@@ -216,6 +218,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -250,6 +253,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -425,7 +429,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -433,13 +437,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
     <col min="2" max="2" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -448,16 +452,16 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="str">
         <f>_xll.s2sub(s2cfg!$A$1,$A$1,A2)</f>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -472,15 +476,15 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
@@ -497,41 +501,41 @@
     <col min="13" max="13" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="str">
         <f>_xll.s2today(-7)</f>
-        <v>2017-05-04</v>
+        <v>2017-05-06</v>
       </c>
       <c r="C1" s="2" t="str">
         <f>_xll.s2today(-6)</f>
-        <v>2017-05-05</v>
+        <v>2017-05-07</v>
       </c>
       <c r="D1" s="2" t="str">
         <f>_xll.s2today(-5)</f>
-        <v>2017-05-06</v>
+        <v>2017-05-08</v>
       </c>
       <c r="E1" s="2" t="str">
         <f>_xll.s2today(-4)</f>
-        <v>2017-05-07</v>
+        <v>2017-05-09</v>
       </c>
       <c r="F1" s="2" t="str">
         <f>_xll.s2today(-3)</f>
-        <v>2017-05-08</v>
+        <v>2017-05-10</v>
       </c>
       <c r="G1" s="2" t="str">
         <f>_xll.s2today(-2)</f>
-        <v>2017-05-09</v>
+        <v>2017-05-11</v>
       </c>
       <c r="H1" s="2" t="str">
         <f>_xll.s2today(-1)</f>
-        <v>2017-05-10</v>
+        <v>2017-05-12</v>
       </c>
       <c r="I1" s="2" t="str">
         <f>_xll.s2today(0)</f>
-        <v>2017-05-11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+        <v>2017-05-13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -541,7 +545,7 @@
       </c>
       <c r="C2" t="str">
         <f>_xll.s2bcache( subs!$A$1,C$1,$A2, subs!$B$2)</f>
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="D2" t="str">
         <f>_xll.s2bcache( subs!$A$1,D$1,$A2, subs!$B$2)</f>
@@ -549,28 +553,28 @@
       </c>
       <c r="E2" t="str">
         <f>_xll.s2bcache( subs!$A$1,E$1,$A2, subs!$B$2)</f>
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="F2" t="str">
         <f>_xll.s2bcache( subs!$A$1,F$1,$A2, subs!$B$2)</f>
-        <v>200</v>
+        <v>2800</v>
       </c>
       <c r="G2" t="str">
         <f>_xll.s2bcache( subs!$A$1,G$1,$A2, subs!$B$2)</f>
-        <v>300</v>
+        <v>10000</v>
       </c>
       <c r="H2" t="str">
         <f>_xll.s2bcache( subs!$A$1,H$1,$A2, subs!$B$2)</f>
-        <v>2800</v>
+        <v>2900</v>
       </c>
       <c r="I2" t="str">
         <f>_xll.s2bcache( subs!$A$1,I$1,$A2, subs!$B$2)</f>
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+        <v>2900</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" t="str">
         <f>_xll.s2bcache( subs!$A$1,B$1,$A3, subs!$B$2)</f>
@@ -578,7 +582,7 @@
       </c>
       <c r="C3" t="str">
         <f>_xll.s2bcache( subs!$A$1,C$1,$A3, subs!$B$2)</f>
-        <v>XLL &amp; VBA single host</v>
+        <v>Basic single host</v>
       </c>
       <c r="D3" t="str">
         <f>_xll.s2bcache( subs!$A$1,D$1,$A3, subs!$B$2)</f>
@@ -586,7 +590,7 @@
       </c>
       <c r="E3" t="str">
         <f>_xll.s2bcache( subs!$A$1,E$1,$A3, subs!$B$2)</f>
-        <v>Basic single host</v>
+        <v>XLL &amp; VBA single host</v>
       </c>
       <c r="F3" t="str">
         <f>_xll.s2bcache( subs!$A$1,F$1,$A3, subs!$B$2)</f>
@@ -594,7 +598,7 @@
       </c>
       <c r="G3" t="str">
         <f>_xll.s2bcache( subs!$A$1,G$1,$A3, subs!$B$2)</f>
-        <v>XLL &amp; VBA single host</v>
+        <v>XLL, VBA &amp; RTD single host</v>
       </c>
       <c r="H3" t="str">
         <f>_xll.s2bcache( subs!$A$1,H$1,$A3, subs!$B$2)</f>
@@ -602,12 +606,12 @@
       </c>
       <c r="I3" t="str">
         <f>_xll.s2bcache( subs!$A$1,I$1,$A3, subs!$B$2)</f>
-        <v>XLL, VBA &amp; RTD single host</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+        <v>Basic single host</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" t="str">
         <f>_xll.s2bcache( subs!$A$1,B$1,$A4, subs!$B$2)</f>
@@ -642,9 +646,9 @@
         <v>month</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" t="str">
         <f>_xll.s2bcache( subs!$A$1,B$1,$A5, subs!$B$2)</f>
@@ -679,9 +683,9 @@
         <v>USD</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" t="str">
         <f>_xll.s2bcache( subs!$A$1,B$1,$A6, subs!$B$2)</f>
@@ -689,7 +693,7 @@
       </c>
       <c r="C6" t="str">
         <f>_xll.s2bcache( subs!$A$1,C$1,$A6, subs!$B$2)</f>
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="D6" t="str">
         <f>_xll.s2bcache( subs!$A$1,D$1,$A6, subs!$B$2)</f>
@@ -697,7 +701,7 @@
       </c>
       <c r="E6" t="str">
         <f>_xll.s2bcache( subs!$A$1,E$1,$A6, subs!$B$2)</f>
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="F6" t="str">
         <f>_xll.s2bcache( subs!$A$1,F$1,$A6, subs!$B$2)</f>
@@ -705,7 +709,7 @@
       </c>
       <c r="G6" t="str">
         <f>_xll.s2bcache( subs!$A$1,G$1,$A6, subs!$B$2)</f>
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="H6" t="str">
         <f>_xll.s2bcache( subs!$A$1,H$1,$A6, subs!$B$2)</f>
@@ -713,7 +717,7 @@
       </c>
       <c r="I6" t="str">
         <f>_xll.s2bcache( subs!$A$1,I$1,$A6, subs!$B$2)</f>
-        <v>400</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -722,15 +726,15 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:M1"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.5703125" customWidth="1"/>
     <col min="2" max="2" width="8.7109375" customWidth="1"/>
@@ -742,7 +746,7 @@
     <col min="11" max="11" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -756,7 +760,7 @@
         <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F1" t="s">
         <v>8</v>
@@ -769,14 +773,14 @@
       </c>
       <c r="I1" s="1" t="str">
         <f>_xll.s2today(-7)</f>
-        <v>2017-05-04</v>
+        <v>2017-05-06</v>
       </c>
       <c r="J1" t="s">
         <v>6</v>
       </c>
       <c r="K1" s="1" t="str">
         <f>_xll.s2today( 0)</f>
-        <v>2017-05-11</v>
+        <v>2017-05-13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>